<commit_message>
Auto Appium Server & Emulator Detector Enhancement
</commit_message>
<xml_diff>
--- a/testdata/MyApplicationTCs.xlsx
+++ b/testdata/MyApplicationTCs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierre.shokry\IdeaProjects\Rain\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E018F4-63FC-4A8A-B820-7CC8809193A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B72B597-3A7D-40CC-BDBD-1750EA010055}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>Select Action on click under Actions and print all the elements in the radio selection list view</t>
   </si>
   <si>
-    <t>Scroll down to the bottom and uncheck the show notification checkbox.</t>
-  </si>
-  <si>
     <t>Select Vibration Strength under behavior and set the vibration strength to 100</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>[PRO] Quick settings</t>
+  </si>
+  <si>
+    <t>Scroll down to the bottom and uncheck the show notification checkbox</t>
   </si>
   <si>
     <t>[PRO] Power menu</t>
@@ -446,7 +446,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -492,7 +492,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -500,7 +500,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +514,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -524,57 +524,57 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>